<commit_message>
Update Literature Matrix UU 2022 (Feb update - 1).xlsx
</commit_message>
<xml_diff>
--- a/LITERATURE REVIEW/Literature Matrix UU 2022 (Feb update - 1).xlsx
+++ b/LITERATURE REVIEW/Literature Matrix UU 2022 (Feb update - 1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/a_w_mwangi_uu_nl/Documents/Documents/GitHub/Renewable_Energy_Integration/LITERATURE REVIEW/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agrippina Mwangi\Documents\GitHub\Renewable_Energy_Integration\LITERATURE REVIEW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{F06087ED-E0F2-4FF2-BC24-2FAC29AE827F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9E0BFA4-BE2B-4998-AF41-16CA8F8F09E1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA30DE0D-B5BA-46A7-8959-710B70E59AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{497C0ADB-D672-4D47-81E2-3B9010C22FDB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{497C0ADB-D672-4D47-81E2-3B9010C22FDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Jan-March 2022" sheetId="1" r:id="rId1"/>
@@ -733,7 +733,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -753,12 +753,6 @@
       <color theme="1"/>
       <name val="Century Gothic"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1269,7 +1263,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>

</xml_diff>